<commit_message>
WIP - cleaning up files
</commit_message>
<xml_diff>
--- a/legacy data/CGS1810 900kcp D9 Legacy.xlsx
+++ b/legacy data/CGS1810 900kcp D9 Legacy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="921" firstSheet="17" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="921" firstSheet="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CGS1810 900kcp D9 Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -305,6 +305,15 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -348,15 +357,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -367,7 +367,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
@@ -645,6 +645,31 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -672,31 +697,12 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="5">
@@ -706,7 +712,757 @@
     <cellStyle name="常规 3 4" xfId="3"/>
     <cellStyle name="Normal 2" xfId="4"/>
   </cellStyles>
-  <dxfs count="517">
+  <dxfs count="602">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -793,231 +1549,331 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4335,281 +5191,281 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6147,8 +7003,8 @@
   </sheetPr>
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView topLeftCell="IQ1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="JJ3" sqref="JJ3"/>
+    <sheetView topLeftCell="IM1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K36" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -6587,7 +7443,7 @@
         </is>
       </c>
       <c r="H3" s="62" t="inlineStr"/>
-      <c r="I3" s="118">
+      <c r="I3" s="101">
         <f t="array" ref="I3">IFERROR(((IF(I5&lt;&gt;"", I5*A5, 0) + SUMPRODUCT(--(I6:I115&lt;&gt;""), I6:I115, (A6:A115-A5:A114)))/1000)/H3, "")</f>
         <v/>
       </c>
@@ -6623,7 +7479,7 @@
         </is>
       </c>
       <c r="T3" s="62" t="inlineStr"/>
-      <c r="U3" s="118">
+      <c r="U3" s="101">
         <f t="array" ref="U3">IFERROR(((IF(U5&lt;&gt;"", U5*M5, 0) + SUMPRODUCT(--(U6:U115&lt;&gt;""), U6:U115, (M6:M115-M5:M114)))/1000)/T3, "")</f>
         <v/>
       </c>
@@ -6774,7 +7630,7 @@
       <c r="I5" t="n">
         <v>2.084999999999937</v>
       </c>
-      <c r="J5" s="119">
+      <c r="J5" s="121">
         <f>I5/F$2</f>
         <v/>
       </c>
@@ -6793,7 +7649,7 @@
       <c r="U5" t="n">
         <v>3.599999999999959</v>
       </c>
-      <c r="V5" s="119">
+      <c r="V5" s="121">
         <f>U5/R$2</f>
         <v/>
       </c>
@@ -6814,7 +7670,7 @@
       <c r="I6" t="n">
         <v>3.089999999999904</v>
       </c>
-      <c r="J6" s="119">
+      <c r="J6" s="121">
         <f>I6/F$2</f>
         <v/>
       </c>
@@ -6833,7 +7689,7 @@
       <c r="U6" t="n">
         <v>3.325000000000067</v>
       </c>
-      <c r="V6" s="119">
+      <c r="V6" s="121">
         <f>U6/R$2</f>
         <v/>
       </c>
@@ -6854,7 +7710,7 @@
       <c r="I7" t="n">
         <v>2.965000000000018</v>
       </c>
-      <c r="J7" s="119">
+      <c r="J7" s="121">
         <f>I7/F$2</f>
         <v/>
       </c>
@@ -6880,7 +7736,7 @@
       <c r="U7" t="n">
         <v>3.364999999999974</v>
       </c>
-      <c r="V7" s="119">
+      <c r="V7" s="121">
         <f>U7/R$2</f>
         <v/>
       </c>
@@ -6908,7 +7764,7 @@
       <c r="I8" t="n">
         <v>3.165000000000084</v>
       </c>
-      <c r="J8" s="119">
+      <c r="J8" s="121">
         <f>I8/F$2</f>
         <v/>
       </c>
@@ -6926,7 +7782,7 @@
       <c r="U8" t="n">
         <v>3.700000000000081</v>
       </c>
-      <c r="V8" s="119">
+      <c r="V8" s="121">
         <f>U8/R$2</f>
         <v/>
       </c>
@@ -6946,7 +7802,7 @@
       <c r="I9" t="n">
         <v>3.195000000000014</v>
       </c>
-      <c r="J9" s="119">
+      <c r="J9" s="121">
         <f>I9/F$2</f>
         <v/>
       </c>
@@ -6964,7 +7820,7 @@
       <c r="U9" t="n">
         <v>3.839999999999932</v>
       </c>
-      <c r="V9" s="119">
+      <c r="V9" s="121">
         <f>U9/R$2</f>
         <v/>
       </c>
@@ -6984,7 +7840,7 @@
       <c r="I10" t="n">
         <v>3.105000000000047</v>
       </c>
-      <c r="J10" s="119">
+      <c r="J10" s="121">
         <f>I10/F$2</f>
         <v/>
       </c>
@@ -7010,7 +7866,7 @@
       <c r="U10" t="n">
         <v>3.190000000000026</v>
       </c>
-      <c r="V10" s="119">
+      <c r="V10" s="121">
         <f>U10/R$2</f>
         <v/>
       </c>
@@ -7038,7 +7894,7 @@
       <c r="I11" t="n">
         <v>3.289999999999971</v>
       </c>
-      <c r="J11" s="119">
+      <c r="J11" s="121">
         <f>I11/F$2</f>
         <v/>
       </c>
@@ -7056,7 +7912,7 @@
       <c r="U11" t="n">
         <v>3.030000000000044</v>
       </c>
-      <c r="V11" s="119">
+      <c r="V11" s="121">
         <f>U11/R$2</f>
         <v/>
       </c>
@@ -7076,7 +7932,7 @@
       <c r="I12" t="n">
         <v>3.279999999999994</v>
       </c>
-      <c r="J12" s="119">
+      <c r="J12" s="121">
         <f>I12/F$2</f>
         <v/>
       </c>
@@ -7094,7 +7950,7 @@
       <c r="U12" t="n">
         <v>3.514999999999979</v>
       </c>
-      <c r="V12" s="119">
+      <c r="V12" s="121">
         <f>U12/R$2</f>
         <v/>
       </c>
@@ -7114,7 +7970,7 @@
       <c r="I13" t="n">
         <v>3.329999999999878</v>
       </c>
-      <c r="J13" s="119">
+      <c r="J13" s="121">
         <f>I13/F$2</f>
         <v/>
       </c>
@@ -7140,7 +7996,7 @@
       <c r="U13" t="n">
         <v>3.379999999999939</v>
       </c>
-      <c r="V13" s="119">
+      <c r="V13" s="121">
         <f>U13/R$2</f>
         <v/>
       </c>
@@ -7168,7 +8024,7 @@
       <c r="I14" t="n">
         <v>3.354999999999997</v>
       </c>
-      <c r="J14" s="119">
+      <c r="J14" s="121">
         <f>I14/F$2</f>
         <v/>
       </c>
@@ -7186,7 +8042,7 @@
       <c r="U14" t="n">
         <v>3.220000000000134</v>
       </c>
-      <c r="V14" s="119">
+      <c r="V14" s="121">
         <f>U14/R$2</f>
         <v/>
       </c>
@@ -7210,7 +8066,7 @@
       <c r="I15" t="n">
         <v>3.200000000000003</v>
       </c>
-      <c r="J15" s="119">
+      <c r="J15" s="121">
         <f>I15/F$2</f>
         <v/>
       </c>
@@ -7232,549 +8088,549 @@
       <c r="U15" t="n">
         <v>2.699999999999925</v>
       </c>
-      <c r="V15" s="119">
+      <c r="V15" s="121">
         <f>U15/R$2</f>
         <v/>
       </c>
     </row>
     <row r="16">
-      <c r="J16" s="119" t="n"/>
-      <c r="V16" s="119" t="n"/>
+      <c r="J16" s="121" t="n"/>
+      <c r="V16" s="121" t="n"/>
     </row>
     <row r="17">
-      <c r="J17" s="119" t="n"/>
-      <c r="V17" s="119" t="n"/>
+      <c r="J17" s="121" t="n"/>
+      <c r="V17" s="121" t="n"/>
     </row>
     <row r="18">
-      <c r="J18" s="119" t="n"/>
-      <c r="V18" s="119" t="n"/>
+      <c r="J18" s="121" t="n"/>
+      <c r="V18" s="121" t="n"/>
     </row>
     <row r="19">
-      <c r="J19" s="119" t="n"/>
-      <c r="V19" s="119" t="n"/>
+      <c r="J19" s="121" t="n"/>
+      <c r="V19" s="121" t="n"/>
     </row>
     <row r="20">
-      <c r="J20" s="119" t="n"/>
-      <c r="V20" s="119" t="n"/>
+      <c r="J20" s="121" t="n"/>
+      <c r="V20" s="121" t="n"/>
     </row>
     <row r="21">
-      <c r="J21" s="119" t="n"/>
-      <c r="V21" s="119" t="n"/>
+      <c r="J21" s="121" t="n"/>
+      <c r="V21" s="121" t="n"/>
     </row>
     <row r="22">
-      <c r="J22" s="119" t="n"/>
-      <c r="V22" s="119" t="n"/>
+      <c r="J22" s="121" t="n"/>
+      <c r="V22" s="121" t="n"/>
     </row>
     <row r="23">
-      <c r="J23" s="119" t="n"/>
-      <c r="V23" s="119" t="n"/>
+      <c r="J23" s="121" t="n"/>
+      <c r="V23" s="121" t="n"/>
     </row>
     <row r="24">
-      <c r="J24" s="119" t="n"/>
-      <c r="V24" s="119" t="n"/>
+      <c r="J24" s="121" t="n"/>
+      <c r="V24" s="121" t="n"/>
     </row>
     <row r="25">
-      <c r="J25" s="119" t="n"/>
-      <c r="V25" s="119" t="n"/>
+      <c r="J25" s="121" t="n"/>
+      <c r="V25" s="121" t="n"/>
     </row>
     <row r="26">
-      <c r="J26" s="119" t="n"/>
-      <c r="V26" s="119" t="n"/>
+      <c r="J26" s="121" t="n"/>
+      <c r="V26" s="121" t="n"/>
     </row>
     <row r="27">
-      <c r="J27" s="119" t="n"/>
-      <c r="V27" s="119" t="n"/>
+      <c r="J27" s="121" t="n"/>
+      <c r="V27" s="121" t="n"/>
     </row>
     <row r="28">
-      <c r="J28" s="119" t="n"/>
-      <c r="V28" s="119" t="n"/>
+      <c r="J28" s="121" t="n"/>
+      <c r="V28" s="121" t="n"/>
     </row>
     <row r="29">
-      <c r="J29" s="119" t="n"/>
-      <c r="V29" s="119" t="n"/>
+      <c r="J29" s="121" t="n"/>
+      <c r="V29" s="121" t="n"/>
     </row>
     <row r="30">
-      <c r="J30" s="119" t="n"/>
-      <c r="V30" s="119" t="n"/>
+      <c r="J30" s="121" t="n"/>
+      <c r="V30" s="121" t="n"/>
     </row>
     <row r="31">
-      <c r="J31" s="119" t="n"/>
-      <c r="V31" s="119" t="n"/>
+      <c r="J31" s="121" t="n"/>
+      <c r="V31" s="121" t="n"/>
     </row>
     <row r="32">
-      <c r="J32" s="119" t="n"/>
-      <c r="V32" s="119" t="n"/>
+      <c r="J32" s="121" t="n"/>
+      <c r="V32" s="121" t="n"/>
     </row>
     <row r="33">
-      <c r="J33" s="119" t="n"/>
-      <c r="V33" s="119" t="n"/>
+      <c r="J33" s="121" t="n"/>
+      <c r="V33" s="121" t="n"/>
     </row>
     <row r="34">
-      <c r="J34" s="119" t="n"/>
-      <c r="V34" s="119" t="n"/>
+      <c r="J34" s="121" t="n"/>
+      <c r="V34" s="121" t="n"/>
     </row>
     <row r="35">
-      <c r="J35" s="119" t="n"/>
-      <c r="V35" s="119" t="n"/>
+      <c r="J35" s="121" t="n"/>
+      <c r="V35" s="121" t="n"/>
     </row>
     <row r="36">
-      <c r="J36" s="119" t="n"/>
-      <c r="V36" s="119" t="n"/>
+      <c r="J36" s="121" t="n"/>
+      <c r="V36" s="121" t="n"/>
     </row>
     <row r="37">
-      <c r="J37" s="119" t="n"/>
-      <c r="V37" s="119" t="n"/>
+      <c r="J37" s="121" t="n"/>
+      <c r="V37" s="121" t="n"/>
     </row>
     <row r="38">
-      <c r="J38" s="119" t="n"/>
-      <c r="V38" s="119" t="n"/>
+      <c r="J38" s="121" t="n"/>
+      <c r="V38" s="121" t="n"/>
     </row>
     <row r="39">
-      <c r="J39" s="119" t="n"/>
-      <c r="V39" s="119" t="n"/>
+      <c r="J39" s="121" t="n"/>
+      <c r="V39" s="121" t="n"/>
     </row>
     <row r="40">
-      <c r="J40" s="119" t="n"/>
-      <c r="V40" s="119" t="n"/>
+      <c r="J40" s="121" t="n"/>
+      <c r="V40" s="121" t="n"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K7:K115">
-    <cfRule type="cellIs" priority="139" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="139" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="138" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="138" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="140" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="140" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:L115">
-    <cfRule type="cellIs" priority="136" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="136" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="137" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="137" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7:W115">
-    <cfRule type="cellIs" priority="95" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="95" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="94" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="94" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="93" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="93" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X7:X115">
-    <cfRule type="cellIs" priority="92" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="92" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="91" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="91" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI7:AI115">
-    <cfRule type="cellIs" priority="110" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="110" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="109" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="109" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="108" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="108" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ7:AJ115">
-    <cfRule type="cellIs" priority="107" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="107" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="106" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="106" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU7:AU115">
-    <cfRule type="cellIs" priority="105" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="105" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="104" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="104" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="103" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="103" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV7:AV115">
-    <cfRule type="cellIs" priority="102" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="102" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="101" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="101" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG7:BG115">
-    <cfRule type="cellIs" priority="89" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="89" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="88" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="88" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="90" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="90" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH7:BH115">
-    <cfRule type="cellIs" priority="87" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="87" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="86" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="86" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS7:BS115">
-    <cfRule type="cellIs" priority="84" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="84" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="85" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="85" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="83" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="83" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT7:BT115">
-    <cfRule type="cellIs" priority="82" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="82" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="81" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="81" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CE7:CE115">
-    <cfRule type="cellIs" priority="80" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="80" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="79" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="79" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="78" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="78" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF7:CF115">
-    <cfRule type="cellIs" priority="77" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="77" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="76" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="76" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ7:CQ115">
-    <cfRule type="cellIs" priority="75" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="75" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="74" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="74" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="73" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="73" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CR7:CR115">
-    <cfRule type="cellIs" priority="72" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="72" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="71" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="71" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DC7:DC115">
-    <cfRule type="cellIs" priority="69" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="69" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="70" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="70" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="68" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="68" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DD7:DD115">
-    <cfRule type="cellIs" priority="67" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="67" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="66" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="66" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DO7:DO115">
-    <cfRule type="cellIs" priority="65" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="65" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="64" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="64" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="63" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="63" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DP7:DP115">
-    <cfRule type="cellIs" priority="62" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="62" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="61" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="61" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EA7:EA115">
-    <cfRule type="cellIs" priority="58" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="58" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="59" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="59" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="60" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="60" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EB7:EB115">
-    <cfRule type="cellIs" priority="56" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="56" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="57" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="57" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM7:EM115">
-    <cfRule type="cellIs" priority="55" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="55" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="54" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="54" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="53" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="53" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EN7:EN115">
-    <cfRule type="cellIs" priority="51" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="51" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="52" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="52" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EY7:EY115">
-    <cfRule type="cellIs" priority="50" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="50" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="49" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="49" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="48" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="48" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EZ7:EZ115">
-    <cfRule type="cellIs" priority="47" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="47" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="46" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="46" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK7:FK115">
-    <cfRule type="cellIs" priority="45" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="45" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="43" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="43" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="44" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="44" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL7:FL115">
-    <cfRule type="cellIs" priority="42" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="42" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="41" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="41" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FW7:FW115">
-    <cfRule type="cellIs" priority="40" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="40" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="39" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="39" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="38" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="38" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FX7:FX115">
-    <cfRule type="cellIs" priority="37" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="37" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="36" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="36" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GI7:GI115">
-    <cfRule type="cellIs" priority="35" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="35" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="34" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="34" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="33" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="33" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GJ7:GJ115">
-    <cfRule type="cellIs" priority="32" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="32" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="31" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="31" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GU7:GU115">
-    <cfRule type="cellIs" priority="29" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="29" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="28" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="28" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="30" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="30" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GV7:GV115">
-    <cfRule type="cellIs" priority="27" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="27" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="26" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="26" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG7:HG115">
-    <cfRule type="cellIs" priority="25" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="25" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="24" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="24" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="23" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="23" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH7:HH115">
-    <cfRule type="cellIs" priority="22" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="22" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="21" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="21" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HS7:HS115">
-    <cfRule type="cellIs" priority="20" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="20" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="19" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="19" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="18" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="18" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HT7:HT115">
-    <cfRule type="cellIs" priority="17" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="17" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="16" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="16" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IE7:IE115">
-    <cfRule type="cellIs" priority="14" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="14" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="15" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="15" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="13" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="13" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IF7:IF115">
-    <cfRule type="cellIs" priority="12" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="12" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="11" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IQ7:IQ115">
-    <cfRule type="cellIs" priority="10" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="10" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="9" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="8" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IR7:IR115">
-    <cfRule type="cellIs" priority="7" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="7" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="6" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="6" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JC7:JC115">
-    <cfRule type="cellIs" priority="5" operator="lessThan" dxfId="11">
+    <cfRule type="cellIs" priority="5" operator="lessThan" dxfId="2">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="between" dxfId="12">
+    <cfRule type="cellIs" priority="4" operator="between" dxfId="3">
       <formula>0.05</formula>
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="3" operator="greaterThan" dxfId="0">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JD7:JD115">
-    <cfRule type="cellIs" priority="2" operator="lessThan" dxfId="9">
+    <cfRule type="cellIs" priority="2" operator="lessThan" dxfId="0">
       <formula>$L$2-$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="1" operator="greaterThan" dxfId="9">
+    <cfRule type="cellIs" priority="1" operator="greaterThan" dxfId="0">
       <formula>$L$2+$L$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>